<commit_message>
♻️refactor: update Excel worksheet validation
</commit_message>
<xml_diff>
--- a/public/planilha-modelo-lds.xlsx
+++ b/public/planilha-modelo-lds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marke\Documents\fatec\EstoqueLDS_2\back-api-consulta-inversores\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD8468A4-39EA-441D-91CE-1B81D5BBB64C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C4415F-66BB-43A4-876C-22FA0F55EA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{CAEE7D65-4579-49FA-BC9B-6C124AAF7E89}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Inversor" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Painel!$C$1:$C$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Painel!$C$1:$C$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
-  <si>
-    <t>Inversor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>marca</t>
   </si>
@@ -58,33 +55,6 @@
   </si>
   <si>
     <t>tensao</t>
-  </si>
-  <si>
-    <t>JRE</t>
-  </si>
-  <si>
-    <t>ROE</t>
-  </si>
-  <si>
-    <t>RENES</t>
-  </si>
-  <si>
-    <t>OL3</t>
-  </si>
-  <si>
-    <t>Não existo ainda</t>
-  </si>
-  <si>
-    <t>oioioioioioioioo</t>
-  </si>
-  <si>
-    <t>cas</t>
-  </si>
-  <si>
-    <t>aic</t>
-  </si>
-  <si>
-    <t>ol3</t>
   </si>
 </sst>
 </file>
@@ -132,43 +102,43 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -184,26 +154,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{389E950D-35EB-433D-93C0-BA5D41CEF62E}" name="Tabela1" displayName="Tabela1" ref="A1:D4" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{389E950D-35EB-433D-93C0-BA5D41CEF62E}" name="Tabela1" displayName="Tabela1" ref="A1:D25" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{4AD928B1-0268-4F17-9EB9-8FA28BA35254}" name="marca" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{ACF10685-C9FF-45E8-9E37-71DCF89FAE16}" name="modelo" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{71A9EDDE-E807-4957-AF5C-A34BB9DDEF24}" name="codigoDeBarras" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{802A54BC-3B50-45F1-AF9A-B1430C4561B3}" name="potencia" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{4AD928B1-0268-4F17-9EB9-8FA28BA35254}" name="marca" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{ACF10685-C9FF-45E8-9E37-71DCF89FAE16}" name="modelo" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{71A9EDDE-E807-4957-AF5C-A34BB9DDEF24}" name="codigoDeBarras" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{802A54BC-3B50-45F1-AF9A-B1430C4561B3}" name="potencia" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FBC4A135-1357-4F4E-861A-C2063E9C6154}" name="Tabela13" displayName="Tabela13" ref="A1:E4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FBC4A135-1357-4F4E-861A-C2063E9C6154}" name="Tabela13" displayName="Tabela13" ref="A1:E4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:E4" xr:uid="{FBC4A135-1357-4F4E-861A-C2063E9C6154}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8F07D4F1-2ADC-4A92-A852-4D7E8056738E}" name="marca" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{E4CDA199-6582-4FA5-8B09-7AA2134016D9}" name="modelo" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{4F706024-46C4-4BE5-B6EB-AA5755198517}" name="codigoDeBarras" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{4B4155C4-7381-4FB8-9BED-F9A232C5EC01}" name="potencia" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{0D8F5694-79D0-48A6-9578-D17154BF9BFC}" name="tensao" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{8F07D4F1-2ADC-4A92-A852-4D7E8056738E}" name="marca" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{E4CDA199-6582-4FA5-8B09-7AA2134016D9}" name="modelo" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{4F706024-46C4-4BE5-B6EB-AA5755198517}" name="codigoDeBarras" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{4B4155C4-7381-4FB8-9BED-F9A232C5EC01}" name="potencia" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{0D8F5694-79D0-48A6-9578-D17154BF9BFC}" name="tensao" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -526,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0111AE9A-164B-4D1D-BE59-6C0176290453}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -541,63 +511,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="2">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{8FDEF10C-B607-4702-BE3B-715F49BE23F9}">
+  <dataValidations count="2">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valor Duplicado" error="O Código de barra que você entrou já existe cadastrado na planilha" sqref="C1" xr:uid="{DDFF195C-B131-41B7-9473-8B69135332CE}">
       <formula1>"CONT.SE($C$2:$C$1048576;C2)=1"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{6DEB683C-7590-4B30-A557-577172AB0098}">
+      <formula1>COUNTIF($C$2:$C$1020,C2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -609,10 +543,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEFB3A5C-B1BC-4CA2-83D5-15844B35D9BF}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -627,68 +561,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2">
-        <v>55</v>
-      </c>
-      <c r="E2" s="2">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2">
-        <v>431</v>
-      </c>
-      <c r="E3" s="2">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="3" spans="1:5" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="1">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Registro Duplicado" error="Código de Barras que você entrou já está cadastrado na Planilha" sqref="C2:C1048576" xr:uid="{62C7F02E-8B48-4DBF-9513-8BC4AA395DE0}">
-      <formula1>"CONT.SE($C$2:$C$1048576;C2)=1"</formula1>
+      <formula1>COUNTIF($C$2:$C$1000,C2)=1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>